<commit_message>
Unittests von philipp drin und Doku grundstein geschrieben (11 Seiten) bewertung auch noch grob ausgefüllt
</commit_message>
<xml_diff>
--- a/documentation/Bewertung.xlsx
+++ b/documentation/Bewertung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GEL2BH\Documents\DHBW\Programmieren\python_projekt2\PythonPasswordManager\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E9F9C19-03BF-46DB-9052-1997D089CE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D562BB-2921-4DC3-90CA-20BFA353888E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -195,9 +195,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -207,6 +204,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -606,190 +606,190 @@
   <dimension ref="B1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="46.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="3" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="4">
+        <v>29</v>
+      </c>
     </row>
     <row r="4" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="2:7" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="5">
-        <v>8</v>
-      </c>
-      <c r="E12" s="5"/>
+      <c r="D12" s="4">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>5</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4">
+        <v>10</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="4">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4">
+        <v>10</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>4</v>
+      </c>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="4">
         <v>3</v>
       </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="5">
-        <v>10</v>
-      </c>
-      <c r="D14" s="5">
-        <v>9</v>
-      </c>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="5">
-        <v>10</v>
-      </c>
-      <c r="D15" s="5">
-        <v>10</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="5">
-        <v>5</v>
-      </c>
-      <c r="D16" s="5">
-        <v>5</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="5">
-        <v>5</v>
-      </c>
-      <c r="D17" s="5">
-        <v>4</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="5">
-        <v>5</v>
-      </c>
-      <c r="D18" s="5">
-        <v>2</v>
-      </c>
-      <c r="E18" s="5"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="5">
-        <v>3</v>
-      </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="5"/>
+      <c r="E19" s="4"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f>SUM(D12:D19)</f>
-        <v>41</v>
-      </c>
-      <c r="E20" s="6">
+        <v>33</v>
+      </c>
+      <c r="E20" s="5">
         <f>SUM(E12:E19)</f>
         <v>0</v>
       </c>

</xml_diff>